<commit_message>
clean up, instrument, sn, etc
Clean up code, add comments, add instrument and instrument_serial_number
refactor file name generation
</commit_message>
<xml_diff>
--- a/global_attribute_table.xlsx
+++ b/global_attribute_table.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/cloudstor/SAZ/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F6D9E53-F540-5C43-86A4-63C6DE77DD86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0BF801-DA45-D54E-8A23-54741DFEA52A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14140" yWindow="4100" windowWidth="34180" windowHeight="17740" xr2:uid="{AB62E28C-C197-1443-8F5C-081BEC806BA6}"/>
+    <workbookView xWindow="9840" yWindow="3500" windowWidth="29180" windowHeight="19860" xr2:uid="{AB62E28C-C197-1443-8F5C-081BEC806BA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="cdl" localSheetId="0">Sheet1!$B$2:$F$54</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,32 +23,15 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
-<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{05A3D1CE-C6DB-A040-A323-75D2A596189D}" name="cdl" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/pete/cloudstor/SAZ/cdl.txt" tab="0" comma="1">
-      <textFields count="4">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
-      </textFields>
-    </textPr>
-  </connection>
-</connections>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="148">
   <si>
     <t>Oceanographic and meteorological data from the Southern Ocean Time Series observatory in the Southern Ocean southwest of Tasmania.</t>
   </si>
@@ -122,12 +102,6 @@
     <t>McLane-PARFLUX Mark78H-21</t>
   </si>
   <si>
-    <t>McLane sn 11741-01, G500x21 ; IRS controller #1 ; Mclane sn 11649-01, T250x21 ; McLane sn 11640-01, A500x21</t>
-  </si>
-  <si>
-    <t>Oceans-&gt;Ocean Chemistry-&gt;Biogeochemical Cycles; moles_of_nitrate_and_nitrite_per_unit_mass_in_sea_water; moles_of_phosphate_per_unit_mass_in_sea_water; sea water parctical salinity; sample_number; moles_of_silicate_per_unit_mass_in_sea_water; moles_of_inorganic_carbon_per_unit_mass_in_sea_water; sea water temperature; recovered_bag_contents_mass</t>
-  </si>
-  <si>
     <t>http://creativecommons.org/licenses/by/4.0/</t>
   </si>
   <si>
@@ -149,9 +123,6 @@
     <t>Integrated Marine Observing System (IMOS)</t>
   </si>
   <si>
-    <t>http://www.imos.org.au</t>
-  </si>
-  <si>
     <t>SOTS</t>
   </si>
   <si>
@@ -161,21 +132,6 @@
     <t>NetCDF Climate and Forecast (CF) Metadata Convention Standard Name Table 67</t>
   </si>
   <si>
-    <t>2012-08-01T00:00:00Z</t>
-  </si>
-  <si>
-    <t>2013-09-05T00:00:00Z</t>
-  </si>
-  <si>
-    <t>2012-07-18T00:00:00Z</t>
-  </si>
-  <si>
-    <t>2014-02-28T00:00:00Z</t>
-  </si>
-  <si>
-    <t>+/- 95% ci</t>
-  </si>
-  <si>
     <t xml:space="preserve">abstract </t>
   </si>
   <si>
@@ -215,12 +171,6 @@
     <t xml:space="preserve">data_mode </t>
   </si>
   <si>
-    <t xml:space="preserve">deployment_code </t>
-  </si>
-  <si>
-    <t xml:space="preserve">deployment_number </t>
-  </si>
-  <si>
     <t xml:space="preserve">disclaimer </t>
   </si>
   <si>
@@ -233,30 +183,12 @@
     <t xml:space="preserve">featureType </t>
   </si>
   <si>
-    <t xml:space="preserve">geospatial_lat_max </t>
-  </si>
-  <si>
-    <t xml:space="preserve">geospatial_lat_min </t>
-  </si>
-  <si>
     <t xml:space="preserve">geospatial_lat_units </t>
   </si>
   <si>
-    <t xml:space="preserve">geospatial_lon_max </t>
-  </si>
-  <si>
-    <t xml:space="preserve">geospatial_lon_min </t>
-  </si>
-  <si>
     <t xml:space="preserve">geospatial_lon_units </t>
   </si>
   <si>
-    <t xml:space="preserve">geospatial_vertical_max </t>
-  </si>
-  <si>
-    <t xml:space="preserve">geospatial_vertical_min </t>
-  </si>
-  <si>
     <t xml:space="preserve">geospatial_vertical_positive </t>
   </si>
   <si>
@@ -272,9 +204,6 @@
     <t xml:space="preserve">instrument </t>
   </si>
   <si>
-    <t xml:space="preserve">instrument_serial_number </t>
-  </si>
-  <si>
     <t xml:space="preserve">keywords </t>
   </si>
   <si>
@@ -317,24 +246,9 @@
     <t xml:space="preserve">standard_name_vocabulary </t>
   </si>
   <si>
-    <t xml:space="preserve">time_coverage_start </t>
-  </si>
-  <si>
-    <t xml:space="preserve">time_coverage_end </t>
-  </si>
-  <si>
-    <t xml:space="preserve">time_deployment_start </t>
-  </si>
-  <si>
-    <t xml:space="preserve">time_deployment_end </t>
-  </si>
-  <si>
     <t xml:space="preserve">title </t>
   </si>
   <si>
-    <t xml:space="preserve">uncertainty </t>
-  </si>
-  <si>
     <t>deployment</t>
   </si>
   <si>
@@ -350,12 +264,6 @@
     <t>*</t>
   </si>
   <si>
-    <t>GENERATED</t>
-  </si>
-  <si>
-    <t>Any users of IMOS data are required to clearly acknowledge the source of the material derived from IMOS in the format: Data was sourced from the Integrated Marine Observing System (IMOS) - IMOS is a national collaborative research infrastructure  supported by the Australian Government."If relevant  also credit other organisations involved in collection of this particular datastream (as listed in credit in the metadata record)."</t>
-  </si>
-  <si>
     <t>Data, products and services from IMOS are provided "as is" without any warranty as to fitness for a particular purpose.</t>
   </si>
   <si>
@@ -392,17 +300,230 @@
     <t>http://www.cmar.csiro.au/data/trawler/survey_details.cfm?survey=IN2017_V02</t>
   </si>
   <si>
-    <t>SAZ47-19-2017</t>
-  </si>
-  <si>
     <t>http://www.cmar.csiro.au/data/trawler/survey_details.cfm?survey=IN2018_V02</t>
+  </si>
+  <si>
+    <t>contributor_role</t>
+  </si>
+  <si>
+    <t>Cathryn Wynn-Edwards</t>
+  </si>
+  <si>
+    <t>data analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contributor_name </t>
+  </si>
+  <si>
+    <t>Oceans-&gt;Ocean Chemistry-&gt;Biogeochemical Cycles; mass_flux; SAL_BRINE; pH_BRINE; PC_mass_flux; PN_mass_flux; POC_mass_flux; PIC_mass_flux; BSi_mass_flux</t>
+  </si>
+  <si>
+    <t>comment_uncertainty</t>
+  </si>
+  <si>
+    <t>Mass flux uncertainty estimates are based on weighing errors only (uniformly 0.06%), and do not include sample splitting errors (~3%) or trap collection efficiency variations. Chemical component flux uncertainty estimates combine the mass flux uncertainty and the analytical uncertainty for the component, based on variations in working standards and duplicate samples over long periods. These are uniformly 1.9% for PIC, 2.8% for POC, 2.1% for PC, 3.8% for PN, and 4.9% for BSi.  All uncertainty estimates are 95% confidence intervals (1.96 standard deviations). Further details are available in Wynn-Edwards et al., 2020</t>
+  </si>
+  <si>
+    <t>https://www.cmar.csiro.au/data/trawler/survey_details.cfm?survey=IN2018_V02</t>
+  </si>
+  <si>
+    <t>https://www.cmar.csiro.au/data/trawler/survey_details.cfm?survey=IN2019_V02</t>
+  </si>
+  <si>
+    <t>Any users of IMOS data are required to clearly acknowledge the source of the material derived from IMOS in the format: "Data was sourced from the Integrated Marine Observing System (IMOS) - IMOS is a national collaborative research infrastructure, supported by the Australian Government."</t>
+  </si>
+  <si>
+    <t>SAZ47-20-2018</t>
+  </si>
+  <si>
+    <t>SAZ47-21-2019</t>
+  </si>
+  <si>
+    <t>SAZ46-19-2017</t>
+  </si>
+  <si>
+    <t>https://www.cmar.csiro.au/data/trawler/survey_details.cfm?survey=SS2013_V03</t>
+  </si>
+  <si>
+    <t>https://www.cmar.csiro.au/data/trawler/survey_details.cfm?survey=SS2012_V03</t>
+  </si>
+  <si>
+    <t>SAZ47-14-2011</t>
+  </si>
+  <si>
+    <t>https://www.cmar.csiro.au/data/trawler/survey_details.cfm?survey=SS2011_V03</t>
+  </si>
+  <si>
+    <t>SAZ47-13-2010</t>
+  </si>
+  <si>
+    <t>https://www.cmar.csiro.au/data/trawler/survey_details.cfm?survey=SS2010_V07</t>
+  </si>
+  <si>
+    <t>SAZ47-12-2009</t>
+  </si>
+  <si>
+    <t>https://www.cmar.csiro.au/data/trawler/survey_details.cfm?survey=SS2009_V04</t>
+  </si>
+  <si>
+    <t>SAZ45-11-2008</t>
+  </si>
+  <si>
+    <t>AA08/09vtrials</t>
+  </si>
+  <si>
+    <t>SAZ54-10-2006</t>
+  </si>
+  <si>
+    <t>SAZ47-9b-2006</t>
+  </si>
+  <si>
+    <t>not recovered</t>
+  </si>
+  <si>
+    <t>AA06_V1.1</t>
+  </si>
+  <si>
+    <t>AA07_V03</t>
+  </si>
+  <si>
+    <t>https://www.cmar.csiro.au/data/trawler/survey_details.cfm?survey=SS200603</t>
+  </si>
+  <si>
+    <t>SAZ47-9a-2005</t>
+  </si>
+  <si>
+    <t>AA05_V02</t>
+  </si>
+  <si>
+    <t>SAZ54-9-2005</t>
+  </si>
+  <si>
+    <t>SAZ47-8-2004</t>
+  </si>
+  <si>
+    <t>SAZ54-8-2004</t>
+  </si>
+  <si>
+    <t>AA04_V01</t>
+  </si>
+  <si>
+    <t>SAZ47-7-2003</t>
+  </si>
+  <si>
+    <t>SAZ54-7-2003</t>
+  </si>
+  <si>
+    <t>AA03_V01</t>
+  </si>
+  <si>
+    <t>SAZ54-6-2002</t>
+  </si>
+  <si>
+    <t>SAZ61-6-2002</t>
+  </si>
+  <si>
+    <t>AA02_V01</t>
+  </si>
+  <si>
+    <t>SAZ61-5-2001</t>
+  </si>
+  <si>
+    <t>AA01_V03</t>
+  </si>
+  <si>
+    <t>SAZ54-5-2001</t>
+  </si>
+  <si>
+    <t>SAZ47-5-2001</t>
+  </si>
+  <si>
+    <t>SAZ54-4-2000</t>
+  </si>
+  <si>
+    <t>AA00_V01</t>
+  </si>
+  <si>
+    <t>SAZ47-4-2000</t>
+  </si>
+  <si>
+    <t>SAZ47-3-1999</t>
+  </si>
+  <si>
+    <t>AA99_V01</t>
+  </si>
+  <si>
+    <t>SAZ54-3-1999</t>
+  </si>
+  <si>
+    <t>SAZ47-2-1998</t>
+  </si>
+  <si>
+    <t>AA97_V06</t>
+  </si>
+  <si>
+    <t>SAZ54-2-1998</t>
+  </si>
+  <si>
+    <t>https://www.cmar.csiro.au/data/trawler/survey_details.cfm?survey=SS199902</t>
+  </si>
+  <si>
+    <t>http://www.imos.org.au http://dx.doi.org/10.26198/5dfad21358a8d</t>
+  </si>
+  <si>
+    <t>comment_data_qc_report</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Wynn-Edwards, CA, Davies, DM, Shadwick, EH, Trull, TW (2020) Southern Ocean Time Series. SOTS Quality assessment and control report. Sediment trap particle fluxes Version 1.0. CSIRO, Australia. DOI: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">10.26198/5dfad21358a8d </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(http://dx.doi.org/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>10.26198/5dfad21358a8d</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.5"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -418,13 +539,65 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF007E9A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11.5"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -436,10 +609,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -449,8 +623,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -464,10 +654,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="cdl" connectionId="1" xr16:uid="{D4E3762E-86A4-9D4C-873D-50264464016B}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -767,13 +953,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53348BFB-8ECF-4745-825D-D0BA3C53E339}">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
@@ -785,27 +971,27 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>0</v>
@@ -813,27 +999,27 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>2</v>
@@ -841,13 +1027,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>3</v>
@@ -855,13 +1041,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>4</v>
@@ -869,13 +1055,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>5</v>
@@ -883,13 +1069,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>6</v>
@@ -897,13 +1083,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>7</v>
@@ -911,13 +1097,13 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>8</v>
@@ -925,719 +1111,1312 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>146</v>
       </c>
       <c r="C11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>9</v>
+        <v>80</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="C12" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="C13" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>11</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
-        <v>13</v>
+      <c r="A16" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>104</v>
-      </c>
-      <c r="D16" s="4">
-        <v>15</v>
+        <v>80</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B17" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>101</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C21" t="s">
-        <v>99</v>
-      </c>
-      <c r="D21" s="4">
-        <v>-46.8371</v>
+        <v>80</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C22" t="s">
-        <v>99</v>
-      </c>
-      <c r="D22" s="4">
-        <v>-46.8371</v>
+        <v>80</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="C23" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B24" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
-        <v>99</v>
-      </c>
-      <c r="D24" s="4">
-        <v>141.67850000000001</v>
+        <v>80</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B25" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="C25" t="s">
-        <v>99</v>
-      </c>
-      <c r="D25" s="4">
-        <v>141.67850000000001</v>
+        <v>80</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B27" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="C27" t="s">
-        <v>99</v>
-      </c>
-      <c r="D27" s="4">
-        <v>3900</v>
+        <v>80</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B28" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>99</v>
-      </c>
-      <c r="D28" s="4">
-        <v>1000</v>
+        <v>80</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B29" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B30" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="C30" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B31" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="C31" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B32" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C32" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B33" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="C33" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B34" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="C34" t="s">
-        <v>99</v>
+        <v>80</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B35" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C35" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B36" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="C36" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B37" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="C37" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B38" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="C38" t="s">
-        <v>104</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>27</v>
+        <v>80</v>
+      </c>
+      <c r="D38" s="4">
+        <v>2</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B39" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="C39" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>1</v>
+        <v>145</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B40" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="C40" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B41" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="C41" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="B42" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C42" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B43" t="s">
+        <v>71</v>
+      </c>
+      <c r="C43" t="s">
+        <v>80</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B45" t="s">
+        <v>85</v>
+      </c>
+      <c r="C45" t="s">
+        <v>80</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B46" t="s">
+        <v>79</v>
+      </c>
+      <c r="C46" t="s">
+        <v>80</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B47" t="s">
+        <v>85</v>
+      </c>
+      <c r="C47" t="s">
+        <v>80</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B48" t="s">
+        <v>79</v>
+      </c>
+      <c r="C48" t="s">
+        <v>80</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B49" t="s">
+        <v>85</v>
+      </c>
+      <c r="C49" t="s">
+        <v>80</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B50" t="s">
+        <v>79</v>
+      </c>
+      <c r="C50" t="s">
+        <v>80</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B51" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" t="s">
+        <v>80</v>
+      </c>
+      <c r="D51" s="13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B52" t="s">
+        <v>79</v>
+      </c>
+      <c r="C52" t="s">
+        <v>80</v>
+      </c>
+      <c r="D52" s="13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B53" t="s">
+        <v>85</v>
+      </c>
+      <c r="C53" t="s">
+        <v>80</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B54" t="s">
+        <v>79</v>
+      </c>
+      <c r="C54" t="s">
+        <v>80</v>
+      </c>
+      <c r="D54" s="13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B55" t="s">
+        <v>85</v>
+      </c>
+      <c r="C55" t="s">
+        <v>80</v>
+      </c>
+      <c r="D55" s="13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B56" t="s">
+        <v>79</v>
+      </c>
+      <c r="C56" t="s">
+        <v>80</v>
+      </c>
+      <c r="D56" s="13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B57" t="s">
+        <v>85</v>
+      </c>
+      <c r="C57" t="s">
+        <v>80</v>
+      </c>
+      <c r="D57" s="13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B58" t="s">
+        <v>79</v>
+      </c>
+      <c r="C58" t="s">
+        <v>80</v>
+      </c>
+      <c r="D58" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B59" t="s">
+        <v>85</v>
+      </c>
+      <c r="C59" t="s">
+        <v>80</v>
+      </c>
+      <c r="D59" s="13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B60" t="s">
+        <v>79</v>
+      </c>
+      <c r="C60" t="s">
+        <v>80</v>
+      </c>
+      <c r="D60" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B61" t="s">
+        <v>85</v>
+      </c>
+      <c r="C61" t="s">
+        <v>80</v>
+      </c>
+      <c r="D61" s="13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B62" t="s">
+        <v>79</v>
+      </c>
+      <c r="C62" t="s">
+        <v>80</v>
+      </c>
+      <c r="D62" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B63" t="s">
+        <v>85</v>
+      </c>
+      <c r="C63" t="s">
+        <v>80</v>
+      </c>
+      <c r="D63" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B64" t="s">
+        <v>79</v>
+      </c>
+      <c r="C64" t="s">
+        <v>80</v>
+      </c>
+      <c r="D64" s="13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B65" t="s">
+        <v>85</v>
+      </c>
+      <c r="C65" t="s">
+        <v>80</v>
+      </c>
+      <c r="D65" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B66" t="s">
+        <v>79</v>
+      </c>
+      <c r="C66" t="s">
+        <v>80</v>
+      </c>
+      <c r="D66" s="13" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>125</v>
+      </c>
+      <c r="B67" t="s">
+        <v>85</v>
+      </c>
+      <c r="C67" t="s">
+        <v>80</v>
+      </c>
+      <c r="D67" s="13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>125</v>
+      </c>
+      <c r="B68" t="s">
+        <v>79</v>
+      </c>
+      <c r="C68" t="s">
+        <v>80</v>
+      </c>
+      <c r="D68" s="13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>126</v>
+      </c>
+      <c r="B69" t="s">
+        <v>85</v>
+      </c>
+      <c r="C69" t="s">
+        <v>80</v>
+      </c>
+      <c r="D69" s="13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>126</v>
+      </c>
+      <c r="B70" t="s">
+        <v>79</v>
+      </c>
+      <c r="C70" t="s">
+        <v>80</v>
+      </c>
+      <c r="D70" s="13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>122</v>
+      </c>
+      <c r="B71" t="s">
+        <v>85</v>
+      </c>
+      <c r="C71" t="s">
+        <v>80</v>
+      </c>
+      <c r="D71" s="13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>122</v>
+      </c>
+      <c r="B72" t="s">
+        <v>79</v>
+      </c>
+      <c r="C72" t="s">
+        <v>80</v>
+      </c>
+      <c r="D72" s="13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>123</v>
+      </c>
+      <c r="B73" t="s">
+        <v>85</v>
+      </c>
+      <c r="C73" t="s">
+        <v>80</v>
+      </c>
+      <c r="D73" s="13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>123</v>
+      </c>
+      <c r="B74" t="s">
+        <v>79</v>
+      </c>
+      <c r="C74" t="s">
+        <v>80</v>
+      </c>
+      <c r="D74" s="13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>119</v>
+      </c>
+      <c r="B75" t="s">
+        <v>85</v>
+      </c>
+      <c r="C75" t="s">
+        <v>80</v>
+      </c>
+      <c r="D75" s="13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>119</v>
+      </c>
+      <c r="B76" t="s">
+        <v>79</v>
+      </c>
+      <c r="C76" t="s">
+        <v>80</v>
+      </c>
+      <c r="D76" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>121</v>
+      </c>
+      <c r="B77" t="s">
+        <v>85</v>
+      </c>
+      <c r="C77" t="s">
+        <v>80</v>
+      </c>
+      <c r="D77" s="13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>121</v>
+      </c>
+      <c r="B78" t="s">
+        <v>79</v>
+      </c>
+      <c r="C78" t="s">
+        <v>80</v>
+      </c>
+      <c r="D78" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>114</v>
+      </c>
+      <c r="B79" t="s">
+        <v>85</v>
+      </c>
+      <c r="C79" t="s">
+        <v>80</v>
+      </c>
+      <c r="D79" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>114</v>
+      </c>
+      <c r="B80" t="s">
+        <v>79</v>
+      </c>
+      <c r="C80" t="s">
+        <v>80</v>
+      </c>
+      <c r="D80" s="13" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>113</v>
+      </c>
+      <c r="B81" t="s">
+        <v>85</v>
+      </c>
+      <c r="C81" t="s">
+        <v>80</v>
+      </c>
+      <c r="D81" s="13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>113</v>
+      </c>
+      <c r="B82" t="s">
+        <v>79</v>
+      </c>
+      <c r="C82" t="s">
+        <v>80</v>
+      </c>
+      <c r="D82" s="13" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>111</v>
+      </c>
+      <c r="B83" t="s">
+        <v>85</v>
+      </c>
+      <c r="C83" t="s">
+        <v>80</v>
+      </c>
+      <c r="D83" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>111</v>
+      </c>
+      <c r="B84" t="s">
+        <v>79</v>
+      </c>
+      <c r="C84" t="s">
+        <v>80</v>
+      </c>
+      <c r="D84" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>109</v>
+      </c>
+      <c r="B85" t="s">
+        <v>85</v>
+      </c>
+      <c r="C85" t="s">
+        <v>80</v>
+      </c>
+      <c r="D85" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>109</v>
+      </c>
+      <c r="B86" t="s">
+        <v>79</v>
+      </c>
+      <c r="C86" t="s">
+        <v>80</v>
+      </c>
+      <c r="D86" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>107</v>
+      </c>
+      <c r="B87" t="s">
+        <v>85</v>
+      </c>
+      <c r="C87" t="s">
+        <v>80</v>
+      </c>
+      <c r="D87" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>107</v>
+      </c>
+      <c r="B88" t="s">
+        <v>79</v>
+      </c>
+      <c r="C88" t="s">
+        <v>80</v>
+      </c>
+      <c r="D88" s="13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>105</v>
+      </c>
+      <c r="B89" t="s">
+        <v>85</v>
+      </c>
+      <c r="C89" t="s">
+        <v>80</v>
+      </c>
+      <c r="D89" s="13" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>105</v>
+      </c>
+      <c r="B90" t="s">
+        <v>79</v>
+      </c>
+      <c r="C90" t="s">
+        <v>80</v>
+      </c>
+      <c r="D90" s="13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" s="12" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>13</v>
+      </c>
+      <c r="B91" t="s">
+        <v>85</v>
+      </c>
+      <c r="C91" t="s">
+        <v>80</v>
+      </c>
+      <c r="D91" s="14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>13</v>
+      </c>
+      <c r="B92" t="s">
+        <v>79</v>
+      </c>
+      <c r="C92" t="s">
+        <v>80</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>82</v>
+      </c>
+      <c r="B93" t="s">
+        <v>85</v>
+      </c>
+      <c r="C93" t="s">
+        <v>80</v>
+      </c>
+      <c r="D93" s="9" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>82</v>
+      </c>
+      <c r="B94" t="s">
+        <v>79</v>
+      </c>
+      <c r="C94" t="s">
+        <v>80</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>84</v>
+      </c>
+      <c r="B95" t="s">
+        <v>85</v>
+      </c>
+      <c r="C95" t="s">
+        <v>80</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>84</v>
+      </c>
+      <c r="B96" t="s">
+        <v>79</v>
+      </c>
+      <c r="C96" t="s">
+        <v>80</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>86</v>
+      </c>
+      <c r="B97" t="s">
+        <v>85</v>
+      </c>
+      <c r="C97" t="s">
+        <v>80</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>86</v>
+      </c>
+      <c r="B98" t="s">
+        <v>79</v>
+      </c>
+      <c r="C98" t="s">
+        <v>80</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B99" t="s">
+        <v>85</v>
+      </c>
+      <c r="C99" t="s">
+        <v>80</v>
+      </c>
+      <c r="D99" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B100" t="s">
+        <v>79</v>
+      </c>
+      <c r="C100" t="s">
+        <v>80</v>
+      </c>
+      <c r="D100" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>85</v>
+      </c>
+      <c r="C101" t="s">
+        <v>80</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>100</v>
+      </c>
+      <c r="B102" t="s">
+        <v>79</v>
+      </c>
+      <c r="C102" t="s">
+        <v>80</v>
+      </c>
+      <c r="D102" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B43" t="s">
-        <v>82</v>
-      </c>
-      <c r="C43" t="s">
-        <v>104</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>101</v>
+      </c>
+      <c r="B103" t="s">
+        <v>85</v>
+      </c>
+      <c r="C103" t="s">
+        <v>80</v>
+      </c>
+      <c r="D103" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B44" t="s">
-        <v>83</v>
-      </c>
-      <c r="C44" t="s">
-        <v>104</v>
-      </c>
-      <c r="D44" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B45" t="s">
-        <v>84</v>
-      </c>
-      <c r="C45" t="s">
-        <v>104</v>
-      </c>
-      <c r="D45" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B46" t="s">
-        <v>85</v>
-      </c>
-      <c r="C46" t="s">
-        <v>104</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B47" t="s">
-        <v>86</v>
-      </c>
-      <c r="C47" t="s">
-        <v>104</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B48" t="s">
-        <v>87</v>
-      </c>
-      <c r="C48" t="s">
-        <v>104</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B49" t="s">
-        <v>88</v>
-      </c>
-      <c r="C49" t="s">
-        <v>99</v>
-      </c>
-      <c r="D49" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B50" t="s">
-        <v>89</v>
-      </c>
-      <c r="C50" t="s">
-        <v>99</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B51" t="s">
-        <v>90</v>
-      </c>
-      <c r="C51" t="s">
-        <v>99</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B52" t="s">
-        <v>91</v>
-      </c>
-      <c r="C52" t="s">
-        <v>99</v>
-      </c>
-      <c r="D52" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B53" t="s">
-        <v>92</v>
-      </c>
-      <c r="C53" t="s">
-        <v>104</v>
-      </c>
-      <c r="D53" s="4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B54" t="s">
-        <v>93</v>
-      </c>
-      <c r="C54" t="s">
-        <v>104</v>
-      </c>
-      <c r="D54" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>13</v>
-      </c>
-      <c r="B55" t="s">
-        <v>103</v>
-      </c>
-      <c r="C55" t="s">
-        <v>104</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>106</v>
-      </c>
-      <c r="B56" t="s">
-        <v>103</v>
-      </c>
-      <c r="C56" t="s">
-        <v>104</v>
-      </c>
-      <c r="D56" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>108</v>
-      </c>
-      <c r="B57" t="s">
-        <v>109</v>
-      </c>
-      <c r="C57" t="s">
-        <v>104</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>110</v>
-      </c>
-      <c r="B58" t="s">
-        <v>109</v>
-      </c>
-      <c r="C58" t="s">
-        <v>104</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" t="s">
-        <v>110</v>
-      </c>
-      <c r="B59" t="s">
-        <v>103</v>
-      </c>
-      <c r="C59" t="s">
-        <v>104</v>
-      </c>
-      <c r="D59" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" t="s">
-        <v>113</v>
-      </c>
-      <c r="B60" t="s">
-        <v>109</v>
-      </c>
-      <c r="C60" t="s">
-        <v>104</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" t="s">
-        <v>113</v>
-      </c>
-      <c r="B61" t="s">
-        <v>103</v>
-      </c>
-      <c r="C61" t="s">
-        <v>104</v>
-      </c>
-      <c r="D61" s="4" t="s">
-        <v>114</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D103" r:id="rId1" xr:uid="{A219C8BE-C520-41E0-ADE3-8E898CB44D2A}"/>
+    <hyperlink ref="D93" r:id="rId2" xr:uid="{1FE2022A-31F1-4A60-AF77-8990993E519E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
version 7 or 2012 data and remove quality_control_set
</commit_message>
<xml_diff>
--- a/global_attribute_table.xlsx
+++ b/global_attribute_table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pete/cloudstor/SAZ/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan079\cloudstor\SAZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0BF801-DA45-D54E-8A23-54741DFEA52A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9620C52-4DE0-4531-919F-E83F54E77B60}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9840" yWindow="3500" windowWidth="29180" windowHeight="19860" xr2:uid="{AB62E28C-C197-1443-8F5C-081BEC806BA6}"/>
+    <workbookView xWindow="9750" yWindow="630" windowWidth="26910" windowHeight="19395" xr2:uid="{AB62E28C-C197-1443-8F5C-081BEC806BA6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="147">
   <si>
     <t>Oceanographic and meteorological data from the Southern Ocean Time Series observatory in the Southern Ocean southwest of Tasmania.</t>
   </si>
@@ -231,9 +231,6 @@
     <t xml:space="preserve">project </t>
   </si>
   <si>
-    <t xml:space="preserve">quality_control_set </t>
-  </si>
-  <si>
     <t xml:space="preserve">references </t>
   </si>
   <si>
@@ -337,9 +334,6 @@
   </si>
   <si>
     <t>SAZ47-21-2019</t>
-  </si>
-  <si>
-    <t>SAZ46-19-2017</t>
   </si>
   <si>
     <t>https://www.cmar.csiro.au/data/trawler/survey_details.cfm?survey=SS2013_V03</t>
@@ -518,6 +512,9 @@
       <t>)</t>
     </r>
   </si>
+  <si>
+    <t>SAZ47-19-2017</t>
+  </si>
 </sst>
 </file>
 
@@ -526,6 +523,13 @@
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -572,13 +576,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -611,33 +608,33 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -953,1468 +950,1454 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53348BFB-8ECF-4745-825D-D0BA3C53E339}">
-  <dimension ref="A1:D103"/>
+  <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:XFD38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.375" customWidth="1"/>
     <col min="4" max="4" width="82" style="4" customWidth="1"/>
-    <col min="5" max="5" width="38.6640625" customWidth="1"/>
-    <col min="6" max="6" width="29.6640625" customWidth="1"/>
+    <col min="5" max="5" width="38.625" customWidth="1"/>
+    <col min="6" max="6" width="29.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
         <v>33</v>
       </c>
       <c r="C2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
         <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
         <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
         <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
         <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
         <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B8" t="s">
         <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B9" t="s">
         <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B10" t="s">
         <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B11" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B13" t="s">
-        <v>90</v>
-      </c>
-      <c r="C13" t="s">
-        <v>80</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
         <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
         <v>43</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B16" t="s">
         <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B17" t="s">
         <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B18" t="s">
         <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B19" t="s">
         <v>47</v>
       </c>
       <c r="C19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B20" t="s">
         <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B21" t="s">
         <v>49</v>
       </c>
       <c r="C21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D21" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B22" t="s">
         <v>50</v>
       </c>
       <c r="C22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B23" t="s">
         <v>51</v>
       </c>
       <c r="C23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B24" t="s">
         <v>52</v>
       </c>
       <c r="C24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B25" t="s">
         <v>53</v>
       </c>
       <c r="C25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
         <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B27" t="s">
         <v>55</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B28" t="s">
         <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B29" t="s">
         <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B30" t="s">
         <v>58</v>
       </c>
       <c r="C30" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B31" t="s">
         <v>59</v>
       </c>
       <c r="C31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D31" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B32" t="s">
         <v>60</v>
       </c>
       <c r="C32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D32" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B33" t="s">
         <v>61</v>
       </c>
       <c r="C33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B34" t="s">
         <v>62</v>
       </c>
       <c r="C34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D34" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B35" t="s">
         <v>63</v>
       </c>
       <c r="C35" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D35" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B36" t="s">
         <v>64</v>
       </c>
       <c r="C36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D36" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B37" t="s">
         <v>65</v>
       </c>
       <c r="C37" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D37" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B38" t="s">
         <v>66</v>
       </c>
       <c r="C38" t="s">
-        <v>80</v>
-      </c>
-      <c r="D38" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B39" t="s">
         <v>67</v>
       </c>
       <c r="C39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B40" t="s">
         <v>68</v>
       </c>
       <c r="C40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B41" t="s">
         <v>69</v>
       </c>
       <c r="C41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B42" t="s">
         <v>70</v>
       </c>
       <c r="C42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B43" t="s">
-        <v>71</v>
-      </c>
-      <c r="C43" t="s">
-        <v>80</v>
-      </c>
-      <c r="D43" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B44" s="6" t="s">
+    <row r="43" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D43" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C44" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B44" t="s">
+        <v>84</v>
+      </c>
+      <c r="C44" t="s">
+        <v>79</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B45" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C45" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D45" s="13" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="46" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>141</v>
       </c>
       <c r="B46" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C46" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B47" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C47" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D47" s="13" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="48" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="B48" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C48" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B49" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C49" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D49" s="13" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>138</v>
       </c>
       <c r="B50" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C50" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D50" s="13" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B51" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C51" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B52" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B53" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C53" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D53" s="13" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B54" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C54" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D54" s="13" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B55" t="s">
+        <v>78</v>
+      </c>
+      <c r="C55" t="s">
+        <v>79</v>
+      </c>
+      <c r="D55" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="11" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="B55" t="s">
-        <v>85</v>
-      </c>
-      <c r="C55" t="s">
-        <v>80</v>
-      </c>
-      <c r="D55" s="13" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="11" t="s">
-        <v>135</v>
-      </c>
       <c r="B56" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D56" s="13" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="11" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="11" t="s">
-        <v>134</v>
-      </c>
       <c r="B57" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C57" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D57" s="13" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B58" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C58" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D58" s="13" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="59" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B59" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D59" s="13" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="11" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B60" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C60" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D60" s="13" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="61" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B61" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C61" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="11" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B62" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C62" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D62" s="13" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B63" t="s">
+        <v>78</v>
+      </c>
+      <c r="C63" t="s">
+        <v>79</v>
+      </c>
+      <c r="D63" s="13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B64" t="s">
+        <v>84</v>
+      </c>
+      <c r="C64" t="s">
+        <v>79</v>
+      </c>
+      <c r="D64" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="B63" t="s">
-        <v>85</v>
-      </c>
-      <c r="C63" t="s">
-        <v>80</v>
-      </c>
-      <c r="D63" s="13" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="B64" t="s">
-        <v>79</v>
-      </c>
-      <c r="C64" t="s">
-        <v>80</v>
-      </c>
-      <c r="D64" s="13" t="s">
+    </row>
+    <row r="65" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="11" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="11" t="s">
-        <v>129</v>
-      </c>
       <c r="B65" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C65" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D65" s="13" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="11" t="s">
-        <v>129</v>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>123</v>
       </c>
       <c r="B66" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C66" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D66" s="13" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>123</v>
+      </c>
+      <c r="B67" t="s">
+        <v>78</v>
+      </c>
+      <c r="C67" t="s">
+        <v>79</v>
+      </c>
+      <c r="D67" s="13" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>124</v>
+      </c>
+      <c r="B68" t="s">
+        <v>84</v>
+      </c>
+      <c r="C68" t="s">
+        <v>79</v>
+      </c>
+      <c r="D68" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="B67" t="s">
-        <v>85</v>
-      </c>
-      <c r="C67" t="s">
-        <v>80</v>
-      </c>
-      <c r="D67" s="13" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>125</v>
-      </c>
-      <c r="B68" t="s">
-        <v>79</v>
-      </c>
-      <c r="C68" t="s">
-        <v>80</v>
-      </c>
-      <c r="D68" s="13" t="s">
+    </row>
+    <row r="69" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>126</v>
-      </c>
       <c r="B69" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C69" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D69" s="13" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B70" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C70" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D70" s="13" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>120</v>
+      </c>
+      <c r="B71" t="s">
+        <v>78</v>
+      </c>
+      <c r="C71" t="s">
+        <v>79</v>
+      </c>
+      <c r="D71" s="13" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>121</v>
+      </c>
+      <c r="B72" t="s">
+        <v>84</v>
+      </c>
+      <c r="C72" t="s">
+        <v>79</v>
+      </c>
+      <c r="D72" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="B71" t="s">
-        <v>85</v>
-      </c>
-      <c r="C71" t="s">
-        <v>80</v>
-      </c>
-      <c r="D71" s="13" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>122</v>
-      </c>
-      <c r="B72" t="s">
-        <v>79</v>
-      </c>
-      <c r="C72" t="s">
-        <v>80</v>
-      </c>
-      <c r="D72" s="13" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B73" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C73" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D73" s="13" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B74" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C74" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D74" s="13" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B75" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C75" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D75" s="13" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>119</v>
       </c>
       <c r="B76" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C76" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D76" s="13" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="77" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B77" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C77" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D77" s="13" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B78" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C78" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D78" s="13" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="79" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>112</v>
+      </c>
+      <c r="B79" t="s">
+        <v>78</v>
+      </c>
+      <c r="C79" t="s">
+        <v>79</v>
+      </c>
+      <c r="D79" s="13" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>111</v>
+      </c>
+      <c r="B80" t="s">
+        <v>84</v>
+      </c>
+      <c r="C80" t="s">
+        <v>79</v>
+      </c>
+      <c r="D80" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="B79" t="s">
-        <v>85</v>
-      </c>
-      <c r="C79" t="s">
-        <v>80</v>
-      </c>
-      <c r="D79" s="13" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>114</v>
-      </c>
-      <c r="B80" t="s">
-        <v>79</v>
-      </c>
-      <c r="C80" t="s">
-        <v>80</v>
-      </c>
-      <c r="D80" s="13" t="s">
+    </row>
+    <row r="81" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>111</v>
+      </c>
+      <c r="B81" t="s">
+        <v>78</v>
+      </c>
+      <c r="C81" t="s">
+        <v>79</v>
+      </c>
+      <c r="D81" s="13" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="81" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>113</v>
-      </c>
-      <c r="B81" t="s">
-        <v>85</v>
-      </c>
-      <c r="C81" t="s">
-        <v>80</v>
-      </c>
-      <c r="D81" s="13" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B82" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C82" t="s">
-        <v>80</v>
-      </c>
-      <c r="D82" s="13" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+      <c r="D82" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B83" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C83" t="s">
-        <v>80</v>
-      </c>
-      <c r="D83" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+      <c r="D83" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B84" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C84" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D84" s="12" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B85" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C85" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D85" s="12" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B86" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C86" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D86" s="12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B87" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C87" t="s">
-        <v>80</v>
-      </c>
-      <c r="D87" s="12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+      <c r="D87" s="13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B88" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C88" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D88" s="13" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B89" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C89" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D89" s="13" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>105</v>
+        <v>13</v>
       </c>
       <c r="B90" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C90" t="s">
-        <v>80</v>
-      </c>
-      <c r="D90" s="13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" s="12" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+      <c r="D90" s="14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>13</v>
       </c>
       <c r="B91" t="s">
+        <v>78</v>
+      </c>
+      <c r="C91" t="s">
+        <v>79</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>81</v>
+      </c>
+      <c r="B92" t="s">
+        <v>84</v>
+      </c>
+      <c r="C92" t="s">
+        <v>79</v>
+      </c>
+      <c r="D92" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>81</v>
+      </c>
+      <c r="B93" t="s">
+        <v>78</v>
+      </c>
+      <c r="C93" t="s">
+        <v>79</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>83</v>
+      </c>
+      <c r="B94" t="s">
+        <v>84</v>
+      </c>
+      <c r="C94" t="s">
+        <v>79</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>83</v>
+      </c>
+      <c r="B95" t="s">
+        <v>78</v>
+      </c>
+      <c r="C95" t="s">
+        <v>79</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>85</v>
       </c>
-      <c r="C91" t="s">
-        <v>80</v>
-      </c>
-      <c r="D91" s="14" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A92" t="s">
-        <v>13</v>
-      </c>
-      <c r="B92" t="s">
-        <v>79</v>
-      </c>
-      <c r="C92" t="s">
-        <v>80</v>
-      </c>
-      <c r="D92" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A93" t="s">
-        <v>82</v>
-      </c>
-      <c r="B93" t="s">
+      <c r="B96" t="s">
+        <v>84</v>
+      </c>
+      <c r="C96" t="s">
+        <v>79</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
         <v>85</v>
       </c>
-      <c r="C93" t="s">
-        <v>80</v>
-      </c>
-      <c r="D93" s="9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A94" t="s">
-        <v>82</v>
-      </c>
-      <c r="B94" t="s">
-        <v>79</v>
-      </c>
-      <c r="C94" t="s">
-        <v>80</v>
-      </c>
-      <c r="D94" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A95" t="s">
-        <v>84</v>
-      </c>
-      <c r="B95" t="s">
-        <v>85</v>
-      </c>
-      <c r="C95" t="s">
-        <v>80</v>
-      </c>
-      <c r="D95" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A96" t="s">
-        <v>84</v>
-      </c>
-      <c r="B96" t="s">
-        <v>79</v>
-      </c>
-      <c r="C96" t="s">
-        <v>80</v>
-      </c>
-      <c r="D96" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
-        <v>86</v>
-      </c>
       <c r="B97" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C97" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D97" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A98" t="s">
-        <v>86</v>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="10" t="s">
+        <v>146</v>
       </c>
       <c r="B98" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C98" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="10" t="s">
-        <v>102</v>
+        <v>146</v>
       </c>
       <c r="B99" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C99" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D99" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A100" s="10" t="s">
-        <v>102</v>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C100" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C101" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D101" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C102" t="s">
-        <v>80</v>
-      </c>
-      <c r="D102" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
-        <v>101</v>
-      </c>
-      <c r="B103" t="s">
-        <v>85</v>
-      </c>
-      <c r="C103" t="s">
-        <v>80</v>
-      </c>
-      <c r="D103" s="9" t="s">
-        <v>98</v>
+        <v>79</v>
+      </c>
+      <c r="D102" s="9" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D103" r:id="rId1" xr:uid="{A219C8BE-C520-41E0-ADE3-8E898CB44D2A}"/>
-    <hyperlink ref="D93" r:id="rId2" xr:uid="{1FE2022A-31F1-4A60-AF77-8990993E519E}"/>
+    <hyperlink ref="D102" r:id="rId1" xr:uid="{A219C8BE-C520-41E0-ADE3-8E898CB44D2A}"/>
+    <hyperlink ref="D92" r:id="rId2" xr:uid="{1FE2022A-31F1-4A60-AF77-8990993E519E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
updated global attributes table
I added the link to SOTS annual reports to the global attribute "reference "
</commit_message>
<xml_diff>
--- a/global_attribute_table.xlsx
+++ b/global_attribute_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universitytasmania-my.sharepoint.com/personal/cathryn_wynnedwards_utas_edu_au/Documents/Documents/GitHub/saz-data-processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{12F1C9AC-E2A6-4BB2-B17F-7142736324D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E9187800-8B54-47CD-89B3-CED5533B3ABD}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{12F1C9AC-E2A6-4BB2-B17F-7142736324D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBE1B063-DEE3-44FF-BC76-6683B77AB271}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AB62E28C-C197-1443-8F5C-081BEC806BA6}"/>
   </bookViews>
@@ -435,9 +435,6 @@
   </si>
   <si>
     <t>https://www.cmar.csiro.au/data/trawler/survey_details.cfm?survey=SS199902</t>
-  </si>
-  <si>
-    <t>http://www.imos.org.au http://dx.doi.org/10.26198/5dfad21358a8d</t>
   </si>
   <si>
     <t>comment_data_qc_report</t>
@@ -696,6 +693,9 @@
   </si>
   <si>
     <t>096U20210414</t>
+  </si>
+  <si>
+    <t>Particle flux QC report: http://www.imos.org.au http://dx.doi.org/10.26198/5dfad21358a8d; SOTS annual reports: https://catalogue-imos.aodn.org.au/geonetwork/srv/eng/catalog.search#/metadata/afc166ce-6b34-44d9-b64c-8bb10fd43a07</t>
   </si>
 </sst>
 </file>
@@ -1222,8 +1222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53348BFB-8ECF-4745-825D-D0BA3C53E339}">
   <dimension ref="A1:D427"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A412" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <selection activeCell="A427" sqref="A427:XFD427"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1345,7 +1345,7 @@
         <v>78</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -1381,13 +1381,13 @@
         <v>74</v>
       </c>
       <c r="B11" t="s">
+        <v>134</v>
+      </c>
+      <c r="C11" t="s">
+        <v>78</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>135</v>
-      </c>
-      <c r="C11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -1765,7 +1765,7 @@
         <v>78</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>134</v>
+        <v>206</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
@@ -1840,7 +1840,7 @@
     </row>
     <row r="44" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B44" t="s">
         <v>83</v>
@@ -1849,15 +1849,15 @@
         <v>78</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="45" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C45" t="s">
         <v>78</v>
@@ -1866,52 +1866,52 @@
     </row>
     <row r="46" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C46" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D46" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="47" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D47" s="13" t="s">
         <v>146</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="D47" s="13" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="48" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C48" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D48" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="49" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C49" s="21" t="s">
         <v>78</v>
@@ -1920,7 +1920,7 @@
     </row>
     <row r="50" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B50" t="s">
         <v>77</v>
@@ -1934,10 +1934,10 @@
     </row>
     <row r="51" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C51" s="21" t="s">
         <v>78</v>
@@ -1945,24 +1945,24 @@
     </row>
     <row r="52" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C52" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D52" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="53" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C53" s="12" t="s">
         <v>78</v>
@@ -1973,24 +1973,24 @@
     </row>
     <row r="54" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C54" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D54" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="55" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B55" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C55" s="38" t="s">
         <v>78</v>
@@ -1999,7 +1999,7 @@
     </row>
     <row r="56" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="40" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B56" s="29" t="s">
         <v>83</v>
@@ -2013,10 +2013,10 @@
     </row>
     <row r="57" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B57" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C57" t="s">
         <v>78</v>
@@ -2025,24 +2025,24 @@
     </row>
     <row r="58" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C58" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D58" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="59" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A59" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C59" s="12" t="s">
         <v>78</v>
@@ -2053,24 +2053,24 @@
     </row>
     <row r="60" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C60" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D60" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="61" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B61" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C61" s="21" t="s">
         <v>78</v>
@@ -2079,7 +2079,7 @@
     </row>
     <row r="62" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B62" t="s">
         <v>77</v>
@@ -2093,10 +2093,10 @@
     </row>
     <row r="63" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B63" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C63" t="s">
         <v>78</v>
@@ -2107,58 +2107,58 @@
     </row>
     <row r="64" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C64" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D64" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="65" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C65" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D65" s="23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="66" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A66" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C66" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D66" s="23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="67" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A67" s="11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B67" s="39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C67" s="39" t="s">
         <v>78</v>
       </c>
       <c r="D67" s="23" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="68" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.35">
@@ -2180,7 +2180,7 @@
         <v>132</v>
       </c>
       <c r="B69" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C69" t="s">
         <v>78</v>
@@ -2192,13 +2192,13 @@
         <v>132</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C70" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D70" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="71" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -2206,7 +2206,7 @@
         <v>132</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C71" s="12" t="s">
         <v>78</v>
@@ -2220,13 +2220,13 @@
         <v>132</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C72" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D72" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="73" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.35">
@@ -2234,7 +2234,7 @@
         <v>132</v>
       </c>
       <c r="B73" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C73" s="21" t="s">
         <v>78</v>
@@ -2260,7 +2260,7 @@
         <v>132</v>
       </c>
       <c r="B75" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C75" t="s">
         <v>78</v>
@@ -2274,13 +2274,13 @@
         <v>132</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C76" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D76" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="77" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -2288,13 +2288,13 @@
         <v>132</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C77" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D77" s="23" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="78" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -2302,13 +2302,13 @@
         <v>132</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C78" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D78" s="23" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="79" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -2316,18 +2316,18 @@
         <v>132</v>
       </c>
       <c r="B79" s="39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C79" s="39" t="s">
         <v>78</v>
       </c>
       <c r="D79" s="23" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="80" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A80" s="40" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B80" s="29" t="s">
         <v>83</v>
@@ -2341,10 +2341,10 @@
     </row>
     <row r="81" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A81" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B81" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C81" t="s">
         <v>78</v>
@@ -2355,24 +2355,24 @@
     </row>
     <row r="82" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A82" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B82" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C82" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D82" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="83" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A83" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B83" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C83" s="12" t="s">
         <v>78</v>
@@ -2383,35 +2383,35 @@
     </row>
     <row r="84" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A84" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B84" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C84" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D84" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="85" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A85" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C85" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D85" s="23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="86" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A86" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B86" t="s">
         <v>77</v>
@@ -2425,10 +2425,10 @@
     </row>
     <row r="87" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A87" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B87" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C87" s="21" t="s">
         <v>78</v>
@@ -2437,24 +2437,24 @@
     </row>
     <row r="88" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A88" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B88" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C88" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D88" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="89" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A89" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B89" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C89" s="12" t="s">
         <v>78</v>
@@ -2465,24 +2465,24 @@
     </row>
     <row r="90" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A90" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B90" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C90" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D90" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="91" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A91" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B91" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C91" s="38" t="s">
         <v>78</v>
@@ -2508,7 +2508,7 @@
         <v>130</v>
       </c>
       <c r="B93" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C93" t="s">
         <v>78</v>
@@ -2522,13 +2522,13 @@
         <v>130</v>
       </c>
       <c r="B94" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C94" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D94" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="95" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -2536,7 +2536,7 @@
         <v>130</v>
       </c>
       <c r="B95" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C95" s="12" t="s">
         <v>78</v>
@@ -2550,13 +2550,13 @@
         <v>130</v>
       </c>
       <c r="B96" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C96" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D96" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="97" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -2564,13 +2564,13 @@
         <v>130</v>
       </c>
       <c r="B97" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C97" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D97" s="23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="98" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -2592,7 +2592,7 @@
         <v>130</v>
       </c>
       <c r="B99" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C99" s="21" t="s">
         <v>78</v>
@@ -2604,13 +2604,13 @@
         <v>130</v>
       </c>
       <c r="B100" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C100" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D100" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="101" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -2618,7 +2618,7 @@
         <v>130</v>
       </c>
       <c r="B101" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C101" s="12" t="s">
         <v>78</v>
@@ -2632,13 +2632,13 @@
         <v>130</v>
       </c>
       <c r="B102" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C102" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D102" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="103" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.35">
@@ -2646,7 +2646,7 @@
         <v>130</v>
       </c>
       <c r="B103" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C103" s="38" t="s">
         <v>78</v>
@@ -2655,7 +2655,7 @@
     </row>
     <row r="104" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A104" s="40" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B104" s="29" t="s">
         <v>83</v>
@@ -2669,10 +2669,10 @@
     </row>
     <row r="105" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A105" s="20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B105" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C105" t="s">
         <v>78</v>
@@ -2681,24 +2681,24 @@
     </row>
     <row r="106" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A106" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B106" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C106" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D106" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="107" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A107" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B107" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C107" s="12" t="s">
         <v>78</v>
@@ -2709,24 +2709,24 @@
     </row>
     <row r="108" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A108" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B108" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C108" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D108" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="109" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A109" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B109" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C109" s="21" t="s">
         <v>78</v>
@@ -2735,7 +2735,7 @@
     </row>
     <row r="110" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A110" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B110" t="s">
         <v>77</v>
@@ -2749,10 +2749,10 @@
     </row>
     <row r="111" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A111" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B111" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C111" t="s">
         <v>78</v>
@@ -2763,24 +2763,24 @@
     </row>
     <row r="112" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A112" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B112" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C112" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D112" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="113" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A113" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B113" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C113" s="12" t="s">
         <v>78</v>
@@ -2791,30 +2791,30 @@
     </row>
     <row r="114" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A114" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B114" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C114" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D114" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="115" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A115" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B115" s="39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C115" s="39" t="s">
         <v>78</v>
       </c>
       <c r="D115" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="116" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.35">
@@ -2836,7 +2836,7 @@
         <v>127</v>
       </c>
       <c r="B117" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C117" t="s">
         <v>78</v>
@@ -2848,13 +2848,13 @@
         <v>127</v>
       </c>
       <c r="B118" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C118" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D118" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="119" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -2862,7 +2862,7 @@
         <v>127</v>
       </c>
       <c r="B119" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C119" s="12" t="s">
         <v>78</v>
@@ -2876,13 +2876,13 @@
         <v>127</v>
       </c>
       <c r="B120" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C120" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D120" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="121" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.35">
@@ -2890,7 +2890,7 @@
         <v>127</v>
       </c>
       <c r="B121" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C121" s="21" t="s">
         <v>78</v>
@@ -2916,7 +2916,7 @@
         <v>127</v>
       </c>
       <c r="B123" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C123" t="s">
         <v>78</v>
@@ -2930,13 +2930,13 @@
         <v>127</v>
       </c>
       <c r="B124" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C124" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D124" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="125" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -2944,7 +2944,7 @@
         <v>127</v>
       </c>
       <c r="B125" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C125" s="12" t="s">
         <v>78</v>
@@ -2958,13 +2958,13 @@
         <v>127</v>
       </c>
       <c r="B126" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C126" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D126" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="127" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -2972,18 +2972,18 @@
         <v>127</v>
       </c>
       <c r="B127" s="39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C127" s="39" t="s">
         <v>78</v>
       </c>
       <c r="D127" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="128" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A128" s="40" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B128" s="29" t="s">
         <v>83</v>
@@ -2997,10 +2997,10 @@
     </row>
     <row r="129" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A129" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B129" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C129" t="s">
         <v>78</v>
@@ -3011,24 +3011,24 @@
     </row>
     <row r="130" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A130" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B130" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C130" t="s">
         <v>78</v>
       </c>
       <c r="D130" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="131" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A131" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B131" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C131" t="s">
         <v>78</v>
@@ -3039,35 +3039,35 @@
     </row>
     <row r="132" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A132" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B132" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C132" t="s">
         <v>78</v>
       </c>
       <c r="D132" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="133" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A133" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B133" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C133" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D133" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="134" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A134" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B134" t="s">
         <v>77</v>
@@ -3081,10 +3081,10 @@
     </row>
     <row r="135" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A135" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B135" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C135" t="s">
         <v>78</v>
@@ -3095,24 +3095,24 @@
     </row>
     <row r="136" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A136" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B136" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C136" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D136" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="137" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A137" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B137" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C137" s="12" t="s">
         <v>78</v>
@@ -3123,30 +3123,30 @@
     </row>
     <row r="138" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A138" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B138" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C138" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D138" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="139" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A139" s="11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B139" s="39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C139" s="39" t="s">
         <v>78</v>
       </c>
       <c r="D139" s="23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="140" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.35">
@@ -3168,7 +3168,7 @@
         <v>126</v>
       </c>
       <c r="B141" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C141" t="s">
         <v>78</v>
@@ -3182,13 +3182,13 @@
         <v>126</v>
       </c>
       <c r="B142" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C142" t="s">
         <v>78</v>
       </c>
       <c r="D142" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="143" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -3196,7 +3196,7 @@
         <v>126</v>
       </c>
       <c r="B143" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C143" t="s">
         <v>78</v>
@@ -3210,13 +3210,13 @@
         <v>126</v>
       </c>
       <c r="B144" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C144" t="s">
         <v>78</v>
       </c>
       <c r="D144" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="145" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -3224,13 +3224,13 @@
         <v>126</v>
       </c>
       <c r="B145" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C145" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D145" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="146" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -3252,7 +3252,7 @@
         <v>126</v>
       </c>
       <c r="B147" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C147" t="s">
         <v>78</v>
@@ -3266,13 +3266,13 @@
         <v>126</v>
       </c>
       <c r="B148" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C148" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D148" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="149" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -3280,7 +3280,7 @@
         <v>126</v>
       </c>
       <c r="B149" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C149" s="12" t="s">
         <v>78</v>
@@ -3294,13 +3294,13 @@
         <v>126</v>
       </c>
       <c r="B150" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C150" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D150" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="151" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -3308,13 +3308,13 @@
         <v>126</v>
       </c>
       <c r="B151" s="39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C151" s="39" t="s">
         <v>78</v>
       </c>
       <c r="D151" s="23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="152" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.35">
@@ -3336,7 +3336,7 @@
         <v>124</v>
       </c>
       <c r="B153" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C153" t="s">
         <v>78</v>
@@ -3350,13 +3350,13 @@
         <v>124</v>
       </c>
       <c r="B154" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C154" t="s">
         <v>78</v>
       </c>
       <c r="D154" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="155" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -3364,7 +3364,7 @@
         <v>124</v>
       </c>
       <c r="B155" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C155" t="s">
         <v>78</v>
@@ -3378,13 +3378,13 @@
         <v>124</v>
       </c>
       <c r="B156" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C156" t="s">
         <v>78</v>
       </c>
       <c r="D156" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="157" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -3392,13 +3392,13 @@
         <v>124</v>
       </c>
       <c r="B157" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C157" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D157" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="158" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -3420,7 +3420,7 @@
         <v>124</v>
       </c>
       <c r="B159" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C159" t="s">
         <v>78</v>
@@ -3434,13 +3434,13 @@
         <v>124</v>
       </c>
       <c r="B160" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C160" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D160" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="161" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -3448,7 +3448,7 @@
         <v>124</v>
       </c>
       <c r="B161" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C161" s="12" t="s">
         <v>78</v>
@@ -3462,13 +3462,13 @@
         <v>124</v>
       </c>
       <c r="B162" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C162" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D162" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="163" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -3476,13 +3476,13 @@
         <v>124</v>
       </c>
       <c r="B163" s="39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C163" s="39" t="s">
         <v>78</v>
       </c>
       <c r="D163" s="23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="164" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.35">
@@ -3504,7 +3504,7 @@
         <v>121</v>
       </c>
       <c r="B165" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C165" t="s">
         <v>78</v>
@@ -3518,13 +3518,13 @@
         <v>121</v>
       </c>
       <c r="B166" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C166" t="s">
         <v>78</v>
       </c>
       <c r="D166" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="167" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -3532,7 +3532,7 @@
         <v>121</v>
       </c>
       <c r="B167" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C167" t="s">
         <v>78</v>
@@ -3546,13 +3546,13 @@
         <v>121</v>
       </c>
       <c r="B168" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C168" t="s">
         <v>78</v>
       </c>
       <c r="D168" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="169" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -3560,13 +3560,13 @@
         <v>121</v>
       </c>
       <c r="B169" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C169" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D169" s="23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="170" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -3588,7 +3588,7 @@
         <v>121</v>
       </c>
       <c r="B171" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C171" t="s">
         <v>78</v>
@@ -3602,13 +3602,13 @@
         <v>121</v>
       </c>
       <c r="B172" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C172" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D172" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="173" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -3616,7 +3616,7 @@
         <v>121</v>
       </c>
       <c r="B173" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C173" s="12" t="s">
         <v>78</v>
@@ -3630,13 +3630,13 @@
         <v>121</v>
       </c>
       <c r="B174" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C174" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D174" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="175" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -3644,13 +3644,13 @@
         <v>121</v>
       </c>
       <c r="B175" s="39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C175" s="39" t="s">
         <v>78</v>
       </c>
       <c r="D175" s="23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="176" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.35">
@@ -3672,7 +3672,7 @@
         <v>122</v>
       </c>
       <c r="B177" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C177" t="s">
         <v>78</v>
@@ -3686,13 +3686,13 @@
         <v>122</v>
       </c>
       <c r="B178" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C178" t="s">
         <v>78</v>
       </c>
       <c r="D178" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="179" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -3700,7 +3700,7 @@
         <v>122</v>
       </c>
       <c r="B179" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C179" t="s">
         <v>78</v>
@@ -3714,13 +3714,13 @@
         <v>122</v>
       </c>
       <c r="B180" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C180" t="s">
         <v>78</v>
       </c>
       <c r="D180" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="181" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -3728,13 +3728,13 @@
         <v>122</v>
       </c>
       <c r="B181" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C181" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D181" s="23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="182" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -3756,13 +3756,13 @@
         <v>122</v>
       </c>
       <c r="B183" t="s">
+        <v>148</v>
+      </c>
+      <c r="C183" t="s">
+        <v>78</v>
+      </c>
+      <c r="D183" s="13" t="s">
         <v>149</v>
-      </c>
-      <c r="C183" t="s">
-        <v>78</v>
-      </c>
-      <c r="D183" s="13" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="184" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -3770,13 +3770,13 @@
         <v>122</v>
       </c>
       <c r="B184" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C184" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D184" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="185" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -3784,13 +3784,13 @@
         <v>122</v>
       </c>
       <c r="B185" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C185" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D185" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="186" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -3798,13 +3798,13 @@
         <v>122</v>
       </c>
       <c r="B186" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C186" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D186" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="187" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -3812,18 +3812,18 @@
         <v>122</v>
       </c>
       <c r="B187" s="39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C187" s="39" t="s">
         <v>78</v>
       </c>
       <c r="D187" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="188" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A188" s="29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B188" s="29" t="s">
         <v>83</v>
@@ -3837,10 +3837,10 @@
     </row>
     <row r="189" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B189" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C189" t="s">
         <v>78</v>
@@ -3851,24 +3851,24 @@
     </row>
     <row r="190" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B190" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C190" t="s">
         <v>78</v>
       </c>
       <c r="D190" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="191" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B191" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C191" t="s">
         <v>78</v>
@@ -3879,35 +3879,35 @@
     </row>
     <row r="192" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B192" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C192" t="s">
         <v>78</v>
       </c>
       <c r="D192" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="193" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B193" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C193" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D193" s="23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="194" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B194" t="s">
         <v>77</v>
@@ -3921,10 +3921,10 @@
     </row>
     <row r="195" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B195" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C195" t="s">
         <v>78</v>
@@ -3935,24 +3935,24 @@
     </row>
     <row r="196" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B196" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C196" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D196" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="197" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B197" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C197" s="12" t="s">
         <v>78</v>
@@ -3963,30 +3963,30 @@
     </row>
     <row r="198" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B198" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C198" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D198" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="199" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B199" s="39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C199" s="39" t="s">
         <v>78</v>
       </c>
       <c r="D199" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="200" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.35">
@@ -4008,7 +4008,7 @@
         <v>119</v>
       </c>
       <c r="B201" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C201" t="s">
         <v>78</v>
@@ -4022,13 +4022,13 @@
         <v>119</v>
       </c>
       <c r="B202" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C202" t="s">
         <v>78</v>
       </c>
       <c r="D202" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="203" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -4036,7 +4036,7 @@
         <v>119</v>
       </c>
       <c r="B203" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C203" t="s">
         <v>78</v>
@@ -4050,13 +4050,13 @@
         <v>119</v>
       </c>
       <c r="B204" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C204" t="s">
         <v>78</v>
       </c>
       <c r="D204" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="205" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -4064,13 +4064,13 @@
         <v>119</v>
       </c>
       <c r="B205" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C205" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D205" s="23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="206" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -4092,7 +4092,7 @@
         <v>119</v>
       </c>
       <c r="B207" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C207" t="s">
         <v>78</v>
@@ -4106,13 +4106,13 @@
         <v>119</v>
       </c>
       <c r="B208" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C208" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D208" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="209" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -4120,7 +4120,7 @@
         <v>119</v>
       </c>
       <c r="B209" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C209" s="12" t="s">
         <v>78</v>
@@ -4134,13 +4134,13 @@
         <v>119</v>
       </c>
       <c r="B210" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C210" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D210" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="211" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -4148,18 +4148,18 @@
         <v>119</v>
       </c>
       <c r="B211" s="39" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C211" s="39" t="s">
         <v>78</v>
       </c>
       <c r="D211" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="212" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A212" s="29" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B212" s="29" t="s">
         <v>83</v>
@@ -4173,10 +4173,10 @@
     </row>
     <row r="213" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B213" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C213" t="s">
         <v>78</v>
@@ -4187,24 +4187,24 @@
     </row>
     <row r="214" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B214" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C214" t="s">
         <v>78</v>
       </c>
       <c r="D214" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="215" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B215" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C215" t="s">
         <v>78</v>
@@ -4215,35 +4215,35 @@
     </row>
     <row r="216" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B216" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C216" t="s">
         <v>78</v>
       </c>
       <c r="D216" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="217" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B217" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C217" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D217" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="218" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B218" t="s">
         <v>77</v>
@@ -4257,10 +4257,10 @@
     </row>
     <row r="219" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B219" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C219" s="21" t="s">
         <v>78</v>
@@ -4269,24 +4269,24 @@
     </row>
     <row r="220" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B220" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C220" t="s">
         <v>78</v>
       </c>
       <c r="D220" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="221" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B221" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C221" t="s">
         <v>78</v>
@@ -4297,24 +4297,24 @@
     </row>
     <row r="222" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B222" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C222" t="s">
         <v>78</v>
       </c>
       <c r="D222" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="223" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B223" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C223" s="38" t="s">
         <v>78</v>
@@ -4340,7 +4340,7 @@
         <v>117</v>
       </c>
       <c r="B225" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C225" t="s">
         <v>78</v>
@@ -4354,13 +4354,13 @@
         <v>117</v>
       </c>
       <c r="B226" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C226" t="s">
         <v>78</v>
       </c>
       <c r="D226" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="227" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -4368,7 +4368,7 @@
         <v>117</v>
       </c>
       <c r="B227" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C227" t="s">
         <v>78</v>
@@ -4382,13 +4382,13 @@
         <v>117</v>
       </c>
       <c r="B228" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C228" t="s">
         <v>78</v>
       </c>
       <c r="D228" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="229" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -4396,13 +4396,13 @@
         <v>117</v>
       </c>
       <c r="B229" s="12" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C229" s="12" t="s">
         <v>78</v>
       </c>
       <c r="D229" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="230" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -4424,7 +4424,7 @@
         <v>117</v>
       </c>
       <c r="B231" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C231" s="21" t="s">
         <v>78</v>
@@ -4436,13 +4436,13 @@
         <v>117</v>
       </c>
       <c r="B232" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C232" t="s">
         <v>78</v>
       </c>
       <c r="D232" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="233" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -4450,7 +4450,7 @@
         <v>117</v>
       </c>
       <c r="B233" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C233" t="s">
         <v>78</v>
@@ -4464,13 +4464,13 @@
         <v>117</v>
       </c>
       <c r="B234" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C234" t="s">
         <v>78</v>
       </c>
       <c r="D234" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="235" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.35">
@@ -4478,7 +4478,7 @@
         <v>117</v>
       </c>
       <c r="B235" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C235" s="38" t="s">
         <v>78</v>
@@ -4487,7 +4487,7 @@
     </row>
     <row r="236" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A236" s="29" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B236" s="29" t="s">
         <v>83</v>
@@ -4501,10 +4501,10 @@
     </row>
     <row r="237" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A237" s="21" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B237" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C237" t="s">
         <v>78</v>
@@ -4513,24 +4513,24 @@
     </row>
     <row r="238" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B238" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C238" t="s">
         <v>78</v>
       </c>
       <c r="D238" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="239" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B239" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C239" t="s">
         <v>78</v>
@@ -4541,24 +4541,24 @@
     </row>
     <row r="240" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B240" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C240" t="s">
         <v>78</v>
       </c>
       <c r="D240" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="241" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B241" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C241" s="21" t="s">
         <v>78</v>
@@ -4567,7 +4567,7 @@
     </row>
     <row r="242" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B242" t="s">
         <v>77</v>
@@ -4581,10 +4581,10 @@
     </row>
     <row r="243" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B243" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C243" t="s">
         <v>78</v>
@@ -4595,58 +4595,58 @@
     </row>
     <row r="244" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B244" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C244" t="s">
         <v>78</v>
       </c>
       <c r="D244" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="245" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B245" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C245" t="s">
         <v>78</v>
       </c>
       <c r="D245" s="18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="246" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B246" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C246" t="s">
         <v>78</v>
       </c>
       <c r="D246" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="247" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B247" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C247" s="25" t="s">
         <v>78</v>
       </c>
       <c r="D247" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="248" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.35">
@@ -4668,7 +4668,7 @@
         <v>116</v>
       </c>
       <c r="B249" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C249" t="s">
         <v>78</v>
@@ -4680,13 +4680,13 @@
         <v>116</v>
       </c>
       <c r="B250" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C250" t="s">
         <v>78</v>
       </c>
       <c r="D250" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="251" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.35">
@@ -4694,7 +4694,7 @@
         <v>116</v>
       </c>
       <c r="B251" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C251" t="s">
         <v>78</v>
@@ -4708,13 +4708,13 @@
         <v>116</v>
       </c>
       <c r="B252" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C252" t="s">
         <v>78</v>
       </c>
       <c r="D252" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="253" spans="1:4" s="21" customFormat="1" x14ac:dyDescent="0.35">
@@ -4722,7 +4722,7 @@
         <v>116</v>
       </c>
       <c r="B253" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C253" s="21" t="s">
         <v>78</v>
@@ -4748,7 +4748,7 @@
         <v>116</v>
       </c>
       <c r="B255" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C255" t="s">
         <v>78</v>
@@ -4762,13 +4762,13 @@
         <v>116</v>
       </c>
       <c r="B256" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C256" t="s">
         <v>78</v>
       </c>
       <c r="D256" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="257" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -4776,7 +4776,7 @@
         <v>116</v>
       </c>
       <c r="B257" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C257" t="s">
         <v>78</v>
@@ -4790,13 +4790,13 @@
         <v>116</v>
       </c>
       <c r="B258" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C258" t="s">
         <v>78</v>
       </c>
       <c r="D258" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="259" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -4804,13 +4804,13 @@
         <v>116</v>
       </c>
       <c r="B259" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C259" s="25" t="s">
         <v>78</v>
       </c>
       <c r="D259" s="23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="260" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.35">
@@ -4832,7 +4832,7 @@
         <v>110</v>
       </c>
       <c r="B261" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C261" t="s">
         <v>78</v>
@@ -4846,13 +4846,13 @@
         <v>110</v>
       </c>
       <c r="B262" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C262" t="s">
         <v>78</v>
       </c>
       <c r="D262" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="263" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -4860,13 +4860,13 @@
         <v>110</v>
       </c>
       <c r="B263" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C263" t="s">
         <v>78</v>
       </c>
       <c r="D263" s="18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="264" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -4874,13 +4874,13 @@
         <v>110</v>
       </c>
       <c r="B264" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C264" t="s">
         <v>78</v>
       </c>
       <c r="D264" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="265" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -4888,13 +4888,13 @@
         <v>110</v>
       </c>
       <c r="B265" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C265" t="s">
         <v>78</v>
       </c>
       <c r="D265" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="266" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -4916,13 +4916,13 @@
         <v>110</v>
       </c>
       <c r="B267" t="s">
+        <v>148</v>
+      </c>
+      <c r="C267" t="s">
+        <v>78</v>
+      </c>
+      <c r="D267" s="13" t="s">
         <v>149</v>
-      </c>
-      <c r="C267" t="s">
-        <v>78</v>
-      </c>
-      <c r="D267" s="13" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="268" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -4930,13 +4930,13 @@
         <v>110</v>
       </c>
       <c r="B268" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C268" t="s">
         <v>78</v>
       </c>
       <c r="D268" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="269" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -4944,13 +4944,13 @@
         <v>110</v>
       </c>
       <c r="B269" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C269" t="s">
         <v>78</v>
       </c>
       <c r="D269" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="270" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -4958,13 +4958,13 @@
         <v>110</v>
       </c>
       <c r="B270" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C270" t="s">
         <v>78</v>
       </c>
       <c r="D270" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="271" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -4972,13 +4972,13 @@
         <v>110</v>
       </c>
       <c r="B271" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C271" s="25" t="s">
         <v>78</v>
       </c>
       <c r="D271" s="13" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="272" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.35">
@@ -5000,7 +5000,7 @@
         <v>109</v>
       </c>
       <c r="B273" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C273" t="s">
         <v>78</v>
@@ -5014,13 +5014,13 @@
         <v>109</v>
       </c>
       <c r="B274" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C274" t="s">
         <v>78</v>
       </c>
       <c r="D274" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="275" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -5028,7 +5028,7 @@
         <v>109</v>
       </c>
       <c r="B275" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C275" t="s">
         <v>78</v>
@@ -5042,13 +5042,13 @@
         <v>109</v>
       </c>
       <c r="B276" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C276" t="s">
         <v>78</v>
       </c>
       <c r="D276" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="277" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -5056,13 +5056,13 @@
         <v>109</v>
       </c>
       <c r="B277" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C277" t="s">
         <v>78</v>
       </c>
       <c r="D277" s="23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="278" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -5084,7 +5084,7 @@
         <v>109</v>
       </c>
       <c r="B279" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C279" t="s">
         <v>78</v>
@@ -5098,13 +5098,13 @@
         <v>109</v>
       </c>
       <c r="B280" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C280" t="s">
         <v>78</v>
       </c>
       <c r="D280" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="281" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -5112,7 +5112,7 @@
         <v>109</v>
       </c>
       <c r="B281" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C281" t="s">
         <v>78</v>
@@ -5126,13 +5126,13 @@
         <v>109</v>
       </c>
       <c r="B282" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C282" t="s">
         <v>78</v>
       </c>
       <c r="D282" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="283" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -5140,18 +5140,18 @@
         <v>109</v>
       </c>
       <c r="B283" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C283" s="25" t="s">
         <v>78</v>
       </c>
       <c r="D283" s="23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="284" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A284" s="29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B284" s="29" t="s">
         <v>83</v>
@@ -5165,10 +5165,10 @@
     </row>
     <row r="285" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B285" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C285" t="s">
         <v>78</v>
@@ -5179,24 +5179,24 @@
     </row>
     <row r="286" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B286" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C286" t="s">
         <v>78</v>
       </c>
       <c r="D286" s="23" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="287" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B287" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C287" t="s">
         <v>78</v>
@@ -5207,35 +5207,35 @@
     </row>
     <row r="288" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B288" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C288" t="s">
         <v>78</v>
       </c>
       <c r="D288" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="289" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B289" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C289" t="s">
         <v>78</v>
       </c>
       <c r="D289" s="23" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="290" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B290" t="s">
         <v>77</v>
@@ -5249,10 +5249,10 @@
     </row>
     <row r="291" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B291" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C291" t="s">
         <v>78</v>
@@ -5263,58 +5263,58 @@
     </row>
     <row r="292" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B292" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C292" t="s">
         <v>78</v>
       </c>
       <c r="D292" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="293" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B293" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C293" t="s">
         <v>78</v>
       </c>
       <c r="D293" s="19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="294" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B294" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C294" t="s">
         <v>78</v>
       </c>
       <c r="D294" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="295" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B295" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C295" s="25" t="s">
         <v>78</v>
       </c>
       <c r="D295" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="296" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.35">
@@ -5336,7 +5336,7 @@
         <v>106</v>
       </c>
       <c r="B297" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C297" t="s">
         <v>78</v>
@@ -5350,13 +5350,13 @@
         <v>106</v>
       </c>
       <c r="B298" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C298" t="s">
         <v>78</v>
       </c>
       <c r="D298" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="299" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -5364,13 +5364,13 @@
         <v>106</v>
       </c>
       <c r="B299" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C299" t="s">
         <v>78</v>
       </c>
       <c r="D299" s="19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="300" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -5378,13 +5378,13 @@
         <v>106</v>
       </c>
       <c r="B300" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C300" t="s">
         <v>78</v>
       </c>
       <c r="D300" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="301" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -5392,13 +5392,13 @@
         <v>106</v>
       </c>
       <c r="B301" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C301" t="s">
         <v>78</v>
       </c>
       <c r="D301" s="16" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="302" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -5420,7 +5420,7 @@
         <v>106</v>
       </c>
       <c r="B303" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C303" t="s">
         <v>78</v>
@@ -5434,13 +5434,13 @@
         <v>106</v>
       </c>
       <c r="B304" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C304" t="s">
         <v>78</v>
       </c>
       <c r="D304" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="305" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -5448,13 +5448,13 @@
         <v>106</v>
       </c>
       <c r="B305" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C305" t="s">
         <v>78</v>
       </c>
       <c r="D305" s="23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="306" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -5462,13 +5462,13 @@
         <v>106</v>
       </c>
       <c r="B306" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C306" t="s">
         <v>78</v>
       </c>
       <c r="D306" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="307" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -5476,13 +5476,13 @@
         <v>106</v>
       </c>
       <c r="B307" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C307" s="25" t="s">
         <v>78</v>
       </c>
       <c r="D307" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="308" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.35">
@@ -5504,7 +5504,7 @@
         <v>104</v>
       </c>
       <c r="B309" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C309" t="s">
         <v>78</v>
@@ -5518,13 +5518,13 @@
         <v>104</v>
       </c>
       <c r="B310" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C310" t="s">
         <v>78</v>
       </c>
       <c r="D310" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="311" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -5532,13 +5532,13 @@
         <v>104</v>
       </c>
       <c r="B311" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C311" t="s">
         <v>78</v>
       </c>
       <c r="D311" s="23" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="312" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -5546,13 +5546,13 @@
         <v>104</v>
       </c>
       <c r="B312" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C312" t="s">
         <v>78</v>
       </c>
       <c r="D312" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="313" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -5560,13 +5560,13 @@
         <v>104</v>
       </c>
       <c r="B313" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C313" t="s">
         <v>78</v>
       </c>
       <c r="D313" s="16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="314" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -5588,7 +5588,7 @@
         <v>104</v>
       </c>
       <c r="B315" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C315" t="s">
         <v>78</v>
@@ -5602,13 +5602,13 @@
         <v>104</v>
       </c>
       <c r="B316" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C316" t="s">
         <v>78</v>
       </c>
       <c r="D316" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="317" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -5616,13 +5616,13 @@
         <v>104</v>
       </c>
       <c r="B317" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C317" t="s">
         <v>78</v>
       </c>
       <c r="D317" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="318" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -5630,13 +5630,13 @@
         <v>104</v>
       </c>
       <c r="B318" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C318" t="s">
         <v>78</v>
       </c>
       <c r="D318" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="319" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -5644,13 +5644,13 @@
         <v>104</v>
       </c>
       <c r="B319" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C319" s="25" t="s">
         <v>78</v>
       </c>
       <c r="D319" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="320" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.35">
@@ -5672,7 +5672,7 @@
         <v>102</v>
       </c>
       <c r="B321" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C321" t="s">
         <v>78</v>
@@ -5686,13 +5686,13 @@
         <v>102</v>
       </c>
       <c r="B322" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C322" t="s">
         <v>78</v>
       </c>
       <c r="D322" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="323" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -5700,13 +5700,13 @@
         <v>102</v>
       </c>
       <c r="B323" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C323" t="s">
         <v>78</v>
       </c>
       <c r="D323" s="23" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="324" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -5714,13 +5714,13 @@
         <v>102</v>
       </c>
       <c r="B324" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C324" t="s">
         <v>78</v>
       </c>
       <c r="D324" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="325" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -5728,13 +5728,13 @@
         <v>102</v>
       </c>
       <c r="B325" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C325" t="s">
         <v>78</v>
       </c>
       <c r="D325" s="16" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="326" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -5756,7 +5756,7 @@
         <v>102</v>
       </c>
       <c r="B327" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C327" t="s">
         <v>78</v>
@@ -5770,13 +5770,13 @@
         <v>102</v>
       </c>
       <c r="B328" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C328" t="s">
         <v>78</v>
       </c>
       <c r="D328" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="329" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -5784,13 +5784,13 @@
         <v>102</v>
       </c>
       <c r="B329" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C329" t="s">
         <v>78</v>
       </c>
       <c r="D329" s="17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="330" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -5798,13 +5798,13 @@
         <v>102</v>
       </c>
       <c r="B330" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C330" t="s">
         <v>78</v>
       </c>
       <c r="D330" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="331" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -5812,13 +5812,13 @@
         <v>102</v>
       </c>
       <c r="B331" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C331" s="25" t="s">
         <v>78</v>
       </c>
       <c r="D331" s="16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="332" spans="1:4" s="34" customFormat="1" x14ac:dyDescent="0.35">
@@ -5840,7 +5840,7 @@
         <v>12</v>
       </c>
       <c r="B333" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C333" t="s">
         <v>78</v>
@@ -5854,13 +5854,13 @@
         <v>12</v>
       </c>
       <c r="B334" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C334" t="s">
         <v>78</v>
       </c>
       <c r="D334" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="335" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -5868,13 +5868,13 @@
         <v>12</v>
       </c>
       <c r="B335" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C335" t="s">
         <v>78</v>
       </c>
       <c r="D335" s="17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="336" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -5882,13 +5882,13 @@
         <v>12</v>
       </c>
       <c r="B336" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C336" t="s">
         <v>78</v>
       </c>
       <c r="D336" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="337" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.35">
@@ -5896,13 +5896,13 @@
         <v>12</v>
       </c>
       <c r="B337" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C337" t="s">
         <v>78</v>
       </c>
       <c r="D337" s="16" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="338" spans="1:4" x14ac:dyDescent="0.35">
@@ -5924,7 +5924,7 @@
         <v>12</v>
       </c>
       <c r="B339" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C339" t="s">
         <v>78</v>
@@ -5938,13 +5938,13 @@
         <v>12</v>
       </c>
       <c r="B340" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C340" t="s">
         <v>78</v>
       </c>
       <c r="D340" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="341" spans="1:4" x14ac:dyDescent="0.35">
@@ -5952,13 +5952,13 @@
         <v>12</v>
       </c>
       <c r="B341" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C341" t="s">
         <v>78</v>
       </c>
       <c r="D341" s="23" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="342" spans="1:4" x14ac:dyDescent="0.35">
@@ -5966,13 +5966,13 @@
         <v>12</v>
       </c>
       <c r="B342" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C342" t="s">
         <v>78</v>
       </c>
       <c r="D342" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="343" spans="1:4" x14ac:dyDescent="0.35">
@@ -5980,13 +5980,13 @@
         <v>12</v>
       </c>
       <c r="B343" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C343" s="25" t="s">
         <v>78</v>
       </c>
       <c r="D343" s="16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="344" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.35">
@@ -6008,7 +6008,7 @@
         <v>80</v>
       </c>
       <c r="B345" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C345" t="s">
         <v>78</v>
@@ -6022,13 +6022,13 @@
         <v>80</v>
       </c>
       <c r="B346" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C346" t="s">
         <v>78</v>
       </c>
       <c r="D346" s="16" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.35">
@@ -6036,13 +6036,13 @@
         <v>80</v>
       </c>
       <c r="B347" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C347" t="s">
         <v>78</v>
       </c>
       <c r="D347" s="16" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="348" spans="1:4" x14ac:dyDescent="0.35">
@@ -6050,13 +6050,13 @@
         <v>80</v>
       </c>
       <c r="B348" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C348" t="s">
         <v>78</v>
       </c>
       <c r="D348" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="349" spans="1:4" x14ac:dyDescent="0.35">
@@ -6064,13 +6064,13 @@
         <v>80</v>
       </c>
       <c r="B349" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C349" t="s">
         <v>78</v>
       </c>
       <c r="D349" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="350" spans="1:4" x14ac:dyDescent="0.35">
@@ -6092,7 +6092,7 @@
         <v>80</v>
       </c>
       <c r="B351" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C351" t="s">
         <v>78</v>
@@ -6106,13 +6106,13 @@
         <v>80</v>
       </c>
       <c r="B352" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C352" t="s">
         <v>78</v>
       </c>
       <c r="D352" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.35">
@@ -6120,13 +6120,13 @@
         <v>80</v>
       </c>
       <c r="B353" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C353" t="s">
         <v>78</v>
       </c>
       <c r="D353" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="354" spans="1:4" x14ac:dyDescent="0.35">
@@ -6134,13 +6134,13 @@
         <v>80</v>
       </c>
       <c r="B354" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C354" t="s">
         <v>78</v>
       </c>
       <c r="D354" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.35">
@@ -6148,13 +6148,13 @@
         <v>80</v>
       </c>
       <c r="B355" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C355" s="25" t="s">
         <v>78</v>
       </c>
       <c r="D355" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="356" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.35">
@@ -6176,7 +6176,7 @@
         <v>82</v>
       </c>
       <c r="B357" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C357" t="s">
         <v>78</v>
@@ -6190,13 +6190,13 @@
         <v>82</v>
       </c>
       <c r="B358" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C358" t="s">
         <v>78</v>
       </c>
       <c r="D358" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.35">
@@ -6204,13 +6204,13 @@
         <v>82</v>
       </c>
       <c r="B359" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C359" t="s">
         <v>78</v>
       </c>
       <c r="D359" s="15" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.35">
@@ -6218,13 +6218,13 @@
         <v>82</v>
       </c>
       <c r="B360" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C360" t="s">
         <v>78</v>
       </c>
       <c r="D360" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="361" spans="1:4" x14ac:dyDescent="0.35">
@@ -6232,13 +6232,13 @@
         <v>82</v>
       </c>
       <c r="B361" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C361" t="s">
         <v>78</v>
       </c>
       <c r="D361" s="15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="362" spans="1:4" x14ac:dyDescent="0.35">
@@ -6260,7 +6260,7 @@
         <v>82</v>
       </c>
       <c r="B363" s="26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C363" s="26" t="s">
         <v>78</v>
@@ -6274,13 +6274,13 @@
         <v>82</v>
       </c>
       <c r="B364" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C364" t="s">
         <v>78</v>
       </c>
       <c r="D364" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="365" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.35">
@@ -6288,13 +6288,13 @@
         <v>82</v>
       </c>
       <c r="B365" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C365" t="s">
         <v>78</v>
       </c>
       <c r="D365" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="366" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.35">
@@ -6302,13 +6302,13 @@
         <v>82</v>
       </c>
       <c r="B366" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C366" t="s">
         <v>78</v>
       </c>
       <c r="D366" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="367" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.35">
@@ -6316,13 +6316,13 @@
         <v>82</v>
       </c>
       <c r="B367" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C367" s="25" t="s">
         <v>78</v>
       </c>
       <c r="D367" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="368" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.35">
@@ -6344,7 +6344,7 @@
         <v>84</v>
       </c>
       <c r="B369" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C369" t="s">
         <v>78</v>
@@ -6358,13 +6358,13 @@
         <v>84</v>
       </c>
       <c r="B370" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C370" t="s">
         <v>78</v>
       </c>
       <c r="D370" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.35">
@@ -6372,13 +6372,13 @@
         <v>84</v>
       </c>
       <c r="B371" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C371" t="s">
         <v>78</v>
       </c>
       <c r="D371" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="372" spans="1:4" x14ac:dyDescent="0.35">
@@ -6386,13 +6386,13 @@
         <v>84</v>
       </c>
       <c r="B372" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C372" t="s">
         <v>78</v>
       </c>
       <c r="D372" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="373" spans="1:4" x14ac:dyDescent="0.35">
@@ -6400,13 +6400,13 @@
         <v>84</v>
       </c>
       <c r="B373" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C373" t="s">
         <v>78</v>
       </c>
       <c r="D373" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.35">
@@ -6428,7 +6428,7 @@
         <v>84</v>
       </c>
       <c r="B375" s="26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C375" s="26" t="s">
         <v>78</v>
@@ -6442,13 +6442,13 @@
         <v>84</v>
       </c>
       <c r="B376" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C376" t="s">
         <v>78</v>
       </c>
       <c r="D376" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="377" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.35">
@@ -6456,13 +6456,13 @@
         <v>84</v>
       </c>
       <c r="B377" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C377" t="s">
         <v>78</v>
       </c>
       <c r="D377" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="378" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.35">
@@ -6470,13 +6470,13 @@
         <v>84</v>
       </c>
       <c r="B378" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C378" t="s">
         <v>78</v>
       </c>
       <c r="D378" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="379" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.35">
@@ -6484,18 +6484,18 @@
         <v>84</v>
       </c>
       <c r="B379" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C379" s="25" t="s">
         <v>78</v>
       </c>
       <c r="D379" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="380" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A380" s="31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B380" s="29" t="s">
         <v>83</v>
@@ -6509,10 +6509,10 @@
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A381" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B381" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C381" t="s">
         <v>78</v>
@@ -6523,63 +6523,63 @@
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A382" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B382" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C382" t="s">
         <v>78</v>
       </c>
       <c r="D382" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A383" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B383" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C383" t="s">
         <v>78</v>
       </c>
       <c r="D383" s="15" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A384" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B384" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C384" t="s">
         <v>78</v>
       </c>
       <c r="D384" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="385" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A385" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B385" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C385" t="s">
         <v>78</v>
       </c>
       <c r="D385" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="386" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A386" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B386" t="s">
         <v>77</v>
@@ -6593,10 +6593,10 @@
     </row>
     <row r="387" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A387" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B387" s="26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C387" s="26" t="s">
         <v>78</v>
@@ -6607,58 +6607,58 @@
     </row>
     <row r="388" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A388" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B388" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C388" t="s">
         <v>78</v>
       </c>
       <c r="D388" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="389" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A389" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B389" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C389" t="s">
         <v>78</v>
       </c>
       <c r="D389" s="28" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="390" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A390" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B390" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C390" t="s">
         <v>78</v>
       </c>
       <c r="D390" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="391" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A391" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B391" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C391" s="25" t="s">
         <v>78</v>
       </c>
       <c r="D391" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="392" spans="1:4" s="29" customFormat="1" x14ac:dyDescent="0.35">
@@ -6680,7 +6680,7 @@
         <v>98</v>
       </c>
       <c r="B393" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C393" t="s">
         <v>78</v>
@@ -6694,13 +6694,13 @@
         <v>98</v>
       </c>
       <c r="B394" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C394" t="s">
         <v>78</v>
       </c>
       <c r="D394" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="395" spans="1:4" x14ac:dyDescent="0.35">
@@ -6708,13 +6708,13 @@
         <v>98</v>
       </c>
       <c r="B395" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C395" t="s">
         <v>78</v>
       </c>
       <c r="D395" s="23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.35">
@@ -6722,13 +6722,13 @@
         <v>98</v>
       </c>
       <c r="B396" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C396" t="s">
         <v>78</v>
       </c>
       <c r="D396" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.35">
@@ -6736,13 +6736,13 @@
         <v>98</v>
       </c>
       <c r="B397" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C397" t="s">
         <v>78</v>
       </c>
       <c r="D397" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="398" spans="1:4" x14ac:dyDescent="0.35">
@@ -6764,7 +6764,7 @@
         <v>98</v>
       </c>
       <c r="B399" s="26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C399" s="26" t="s">
         <v>78</v>
@@ -6778,13 +6778,13 @@
         <v>98</v>
       </c>
       <c r="B400" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C400" t="s">
         <v>78</v>
       </c>
       <c r="D400" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="401" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.35">
@@ -6792,13 +6792,13 @@
         <v>98</v>
       </c>
       <c r="B401" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C401" t="s">
         <v>78</v>
       </c>
       <c r="D401" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="402" spans="1:4" s="26" customFormat="1" x14ac:dyDescent="0.35">
@@ -6806,13 +6806,13 @@
         <v>98</v>
       </c>
       <c r="B402" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C402" t="s">
         <v>78</v>
       </c>
       <c r="D402" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="403" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.35">
@@ -6820,13 +6820,13 @@
         <v>98</v>
       </c>
       <c r="B403" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C403" s="25" t="s">
         <v>78</v>
       </c>
       <c r="D403" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="404" spans="1:4" x14ac:dyDescent="0.35">
@@ -6848,7 +6848,7 @@
         <v>99</v>
       </c>
       <c r="B405" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C405" t="s">
         <v>78</v>
@@ -6862,13 +6862,13 @@
         <v>99</v>
       </c>
       <c r="B406" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C406" t="s">
         <v>78</v>
       </c>
       <c r="D406" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.35">
@@ -6876,13 +6876,13 @@
         <v>99</v>
       </c>
       <c r="B407" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C407" t="s">
         <v>78</v>
       </c>
       <c r="D407" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="408" spans="1:4" x14ac:dyDescent="0.35">
@@ -6890,13 +6890,13 @@
         <v>99</v>
       </c>
       <c r="B408" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C408" t="s">
         <v>78</v>
       </c>
       <c r="D408" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="409" spans="1:4" x14ac:dyDescent="0.35">
@@ -6904,13 +6904,13 @@
         <v>99</v>
       </c>
       <c r="B409" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C409" t="s">
         <v>78</v>
       </c>
       <c r="D409" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="410" spans="1:4" x14ac:dyDescent="0.35">
@@ -6924,7 +6924,7 @@
         <v>78</v>
       </c>
       <c r="D410" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="411" spans="1:4" x14ac:dyDescent="0.35">
@@ -6932,7 +6932,7 @@
         <v>99</v>
       </c>
       <c r="B411" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C411" t="s">
         <v>78</v>
@@ -6946,13 +6946,13 @@
         <v>99</v>
       </c>
       <c r="B412" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C412" t="s">
         <v>78</v>
       </c>
       <c r="D412" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="413" spans="1:4" x14ac:dyDescent="0.35">
@@ -6960,13 +6960,13 @@
         <v>99</v>
       </c>
       <c r="B413" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C413" t="s">
         <v>78</v>
       </c>
       <c r="D413" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="414" spans="1:4" x14ac:dyDescent="0.35">
@@ -6974,13 +6974,13 @@
         <v>99</v>
       </c>
       <c r="B414" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C414" t="s">
         <v>78</v>
       </c>
       <c r="D414" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="415" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.35">
@@ -6988,18 +6988,18 @@
         <v>99</v>
       </c>
       <c r="B415" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C415" s="25" t="s">
         <v>78</v>
       </c>
       <c r="D415" s="41" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="416" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A416" s="42" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B416" t="s">
         <v>83</v>
@@ -7008,15 +7008,15 @@
         <v>78</v>
       </c>
       <c r="D416" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="417" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A417" s="42" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B417" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C417" t="s">
         <v>78</v>
@@ -7027,63 +7027,63 @@
     </row>
     <row r="418" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A418" s="42" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B418" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C418" t="s">
         <v>78</v>
       </c>
       <c r="D418" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="419" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A419" s="42" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B419" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C419" t="s">
         <v>78</v>
       </c>
       <c r="D419" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="420" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A420" s="42" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B420" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C420" t="s">
         <v>78</v>
       </c>
       <c r="D420" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="421" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A421" s="42" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B421" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C421" t="s">
         <v>78</v>
       </c>
       <c r="D421" s="44" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="422" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A422" s="42" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B422" t="s">
         <v>77</v>
@@ -7092,15 +7092,15 @@
         <v>78</v>
       </c>
       <c r="D422" s="43" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="423" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A423" s="42" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B423" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C423" t="s">
         <v>78</v>
@@ -7111,58 +7111,58 @@
     </row>
     <row r="424" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A424" s="42" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B424" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C424" t="s">
         <v>78</v>
       </c>
       <c r="D424" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="425" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A425" s="42" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B425" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C425" t="s">
         <v>78</v>
       </c>
       <c r="D425" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="426" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A426" s="42" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B426" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C426" t="s">
         <v>78</v>
       </c>
       <c r="D426" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="427" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A427" s="39" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B427" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C427" s="25" t="s">
         <v>78</v>
       </c>
       <c r="D427" s="45" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
comment_sample now also added to global attributes list
</commit_message>
<xml_diff>
--- a/global_attribute_table.xlsx
+++ b/global_attribute_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/wyn028_csiro_au/Documents/Documents/GitHub/saz-data-processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="13_ncr:1_{12F1C9AC-E2A6-4BB2-B17F-7142736324D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20081FBB-1636-47D5-9C10-FFD6ABF8A474}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="13_ncr:1_{12F1C9AC-E2A6-4BB2-B17F-7142736324D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{917B9DF2-4B4A-4205-8B3C-B97930D09ADE}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{AB62E28C-C197-1443-8F5C-081BEC806BA6}"/>
   </bookViews>
@@ -1243,8 +1243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53348BFB-8ECF-4745-825D-D0BA3C53E339}">
   <dimension ref="A1:D463"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A446" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+      <selection activeCell="B450" sqref="B450"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -7508,8 +7508,8 @@
         <v>154</v>
       </c>
     </row>
-    <row r="451" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A451" t="s">
+    <row r="451" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A451" s="19" t="s">
         <v>207</v>
       </c>
       <c r="B451" s="19" t="s">

</xml_diff>